<commit_message>
Continued writing, new graph
</commit_message>
<xml_diff>
--- a/data/PROCESSED_responsetimes_results_per_interval.xlsx
+++ b/data/PROCESSED_responsetimes_results_per_interval.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12210" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Laadtijd routes aantal resultat" sheetId="7" r:id="rId1"/>
@@ -6047,10 +6047,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="3"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -6118,82 +6118,911 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Gent Sint Pieters, 4u</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:shade val="76000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Stops liveboard'!$A$3:$A$146</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="144"/>
+                <c:pt idx="0">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10200</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12600</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13200</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13800</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14400</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16200</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>17400</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19200</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>19800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20400</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>21600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>22200</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>22800</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>23400</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>24600</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>25200</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>25800</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>26400</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>27600</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>28200</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>28800</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>29400</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>30600</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>31200</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>31800</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>32400</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>33600</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>34200</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>34800</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>35400</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>36600</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>37200</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>37800</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>38400</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>39000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>40200</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>40800</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>41400</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>42000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>42600</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>43200</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>43800</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>44400</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>45600</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>46200</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>46800</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>47400</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>48000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>48600</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>49200</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>49800</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>50400</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>51000</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>51600</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>52200</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>52800</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>53400</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>54000</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>54600</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>55200</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>55800</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>56400</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>57000</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>57600</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>58200</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>58800</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>59400</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>60600</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>61200</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>61800</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>62400</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>63000</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>63600</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>64200</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>64800</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>65400</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>66000</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>66600</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>67200</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>67800</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>68400</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>69000</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>69600</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>70200</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>70800</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>71400</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>72000</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>72600</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>73200</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>73800</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>74400</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>75600</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>76200</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>76800</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>77400</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>78000</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>78600</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>79200</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>79800</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>80400</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>81000</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>81600</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>82200</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>82800</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>83400</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>84000</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>84600</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>85200</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>85800</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>86400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Stops liveboard'!$A$3:$A$21</c:f>
+              <c:f>'Stops liveboard'!$F$3:$F$146</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="144"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>289</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>473</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>497</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>516</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>528</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>564</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>592</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="104">
                   <c:v>600</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4200</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4800</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5400</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8400</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9600</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10200</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10800</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11400</c:v>
+                <c:pt idx="105">
+                  <c:v>605</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>617</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>622</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>628</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>636</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6201,89 +7030,477 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8C86-4CA4-98DD-028FE3301830}"/>
+              <c16:uniqueId val="{00000011-7D83-42C6-8504-32C6BD45B610}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Gent Sint Pieters, 16u</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:tint val="77000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Stops liveboard'!$AA$3:$AA$21</c:f>
+              <c:f>'Stops liveboard'!$R$3:$R$146</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="144"/>
                 <c:pt idx="0">
-                  <c:v>12.291666666666666</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.166666666666668</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.041666666666668</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27.75</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.125</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.375</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.958333333333336</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45.083333333333336</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48.958333333333336</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54.666666666666664</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>65.25</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>67.833333333333329</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>71.958333333333329</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>75.833333333333329</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>81.541666666666671</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>86.875</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>92.125</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>94.708333333333329</c:v>
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>371</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>393</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>427</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>487</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>533</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>537</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>543</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>572</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6291,7 +7508,485 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-8C86-4CA4-98DD-028FE3301830}"/>
+              <c16:uniqueId val="{00000012-7D83-42C6-8504-32C6BD45B610}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Gent sint pieters, gemiddeld</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Stops liveboard'!$AA$3:$AA$146</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="144"/>
+                <c:pt idx="0">
+                  <c:v>12.291666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.166666666666668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.041666666666668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.958333333333336</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.083333333333336</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48.958333333333336</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67.833333333333329</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>71.958333333333329</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75.833333333333329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>81.541666666666671</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>86.875</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92.125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>94.708333333333329</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>98.833333333333329</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>102.70833333333333</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>108.41666666666667</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>113.75</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>121.58333333333333</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>125.875</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>129.75</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>135.58333333333334</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>140.95833333333334</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>146.29166666666666</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>148.91666666666666</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>153.125</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>157.16666666666666</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>163.08333333333334</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>168.70833333333334</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>174.20833333333334</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>176.875</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>181.25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>185.375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>191.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>197.08333333333334</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>202.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>205.45833333333334</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>209.875</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>220.04166666666666</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>225.70833333333334</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>231.25</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>234.04166666666666</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>238.375</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>242.45833333333334</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>248.41666666666666</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>259.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>262.16666666666669</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>266.45833333333331</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>270.5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>276.45833333333331</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>282.04166666666669</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>287.54166666666669</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>290.20833333333331</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>294.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>298.54166666666669</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>304.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>310.08333333333331</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>315.58333333333331</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>318.20833333333331</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>322.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>326.5</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>332.41666666666669</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>343.5</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>346.16666666666669</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>350.375</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>354.25</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>360.20833333333331</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>365.625</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>371</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>373.54166666666669</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>377.625</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>381.41666666666669</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>387.04166666666669</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>392.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>397.58333333333331</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>399.95833333333331</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>403.91666666666669</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>407.625</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>418.04166666666669</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>423.04166666666669</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>425.25</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>429.125</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>432.79166666666669</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>438.125</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>443.08333333333331</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>448.125</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>450.33333333333331</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>454.29166666666669</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>458.04166666666669</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>463.54166666666669</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>468.54166666666669</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>473.54166666666669</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>475.875</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>479.79166666666669</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>483.625</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>489.125</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>494.04166666666669</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>499.08333333333331</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>501.29166666666669</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>505.20833333333331</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>508.875</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>514.16666666666663</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>519.125</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>524.125</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>526.29166666666663</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>530.16666666666663</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>533.83333333333337</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>539.125</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>544.08333333333337</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>549.08333333333337</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>551.25</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>555.125</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>558.79166666666663</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>564.08333333333337</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>569.04166666666663</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>574.04166666666663</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>576.20833333333337</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>580.08333333333337</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>583.75</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>589</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>593.95833333333337</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>598.95833333333337</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>601.125</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>604.95833333333337</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>608.58333333333337</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>613.75</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>618.58333333333337</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>623.54166666666663</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>625.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>629.5</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>633.08333333333337</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>638.125</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>642.83333333333337</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>647.58333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-7D83-42C6-8504-32C6BD45B610}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6303,9 +7998,1468 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="677362896"/>
         <c:axId val="2112109936"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>Gent Sint Pieters, 10u</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Stops liveboard'!$L$3:$L$146</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="144"/>
+                      <c:pt idx="0">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>53</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>67</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>77</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>86</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>91</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>98</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>104</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>118</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>127</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>136</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>142</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>149</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>155</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>167</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>179</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>191</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>197</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>203</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>208</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>216</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>224</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>230</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>233</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>237</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>241</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>248</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>254</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>261</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>264</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>270</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>276</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>287</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>294</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>306</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>311</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>319</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>330</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>335</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>342</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>345</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>350</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>354</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>360</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>366</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>372</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>374</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>378</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>382</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>388</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>394</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>400</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>402</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>406</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>410</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>416</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>422</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>428</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>430</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>434</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>438</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>443</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>449</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>455</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>457</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>460</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>463</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>466</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>469</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>474</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>475</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>478</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>480</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>481</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>483</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>487</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>487</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>490</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>491</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>493</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>494</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>496</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>505</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>512</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>518</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>520</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>526</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>532</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>538</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>548</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>556</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>561</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>568</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>574</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>582</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>590</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>597</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>602</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>607</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>612</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>618</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>624</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>630</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>632</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>636</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>640</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>646</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>652</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>658</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000013-7D83-42C6-8504-32C6BD45B610}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>Kiewit, 4u</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="plus"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Stops liveboard'!$F$438:$F$581</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="144"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>26</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>50</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>50</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000014-7D83-42C6-8504-32C6BD45B610}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:v>Kiewit, 16u</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="x"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Stops liveboard'!$R$438:$R$581</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="144"/>
+                      <c:pt idx="0">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>13</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>14</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>19</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="41">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="42">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="43">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="44">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="45">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="46">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="47">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="48">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="49">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="50">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="51">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="52">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="53">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="54">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="55">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="56">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="57">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="58">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="59">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="60">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="61">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="62">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="63">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="64">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="65">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="66">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="67">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="68">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="69">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="70">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="71">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="72">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="73">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="74">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="75">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="76">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="77">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="78">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="79">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="80">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="81">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="82">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="83">
+                        <c:v>22</c:v>
+                      </c:pt>
+                      <c:pt idx="84">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="85">
+                        <c:v>23</c:v>
+                      </c:pt>
+                      <c:pt idx="86">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="87">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="88">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="89">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="90">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="91">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="92">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="93">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="94">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="95">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="96">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="97">
+                        <c:v>31</c:v>
+                      </c:pt>
+                      <c:pt idx="98">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="99">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="100">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="101">
+                        <c:v>33</c:v>
+                      </c:pt>
+                      <c:pt idx="102">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="103">
+                        <c:v>34</c:v>
+                      </c:pt>
+                      <c:pt idx="104">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="105">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="106">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="107">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="108">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="109">
+                        <c:v>37</c:v>
+                      </c:pt>
+                      <c:pt idx="110">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="111">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="112">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="113">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="114">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="115">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="116">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="117">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="118">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="119">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="120">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="121">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="122">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="123">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="124">
+                        <c:v>42</c:v>
+                      </c:pt>
+                      <c:pt idx="125">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="126">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="127">
+                        <c:v>43</c:v>
+                      </c:pt>
+                      <c:pt idx="128">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="129">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="130">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="131">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="132">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="133">
+                        <c:v>45</c:v>
+                      </c:pt>
+                      <c:pt idx="134">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="135">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="136">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="137">
+                        <c:v>46</c:v>
+                      </c:pt>
+                      <c:pt idx="138">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="139">
+                        <c:v>47</c:v>
+                      </c:pt>
+                      <c:pt idx="140">
+                        <c:v>48</c:v>
+                      </c:pt>
+                      <c:pt idx="141">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="142">
+                        <c:v>49</c:v>
+                      </c:pt>
+                      <c:pt idx="143">
+                        <c:v>49</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000015-7D83-42C6-8504-32C6BD45B610}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="677362896"/>
@@ -6537,7 +9691,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6726,8 +9880,42 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -9359,7 +12547,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9502,7 +12690,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9298983" cy="6075551"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1">
@@ -21497,8 +24685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>